<commit_message>
subir el cambio de mmb
</commit_message>
<xml_diff>
--- a/booking_codes.xlsx
+++ b/booking_codes.xlsx
@@ -1,41 +1,362 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\playwright-project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77D586F-62F0-457A-AA94-4F354F6366AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="4340" yWindow="2790" windowWidth="16920" windowHeight="10450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Booking Codes" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="110">
+  <si>
+    <t>Booking Code</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>M9WLC</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:37:57</t>
+  </si>
+  <si>
+    <t>M9WLN</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:40:11</t>
+  </si>
+  <si>
+    <t>M9WM3</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:43:18</t>
+  </si>
+  <si>
+    <t>M9WM6</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:43:38</t>
+  </si>
+  <si>
+    <t>M9WM9</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:43:40</t>
+  </si>
+  <si>
+    <t>M9WMB</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:44:01</t>
+  </si>
+  <si>
+    <t>M9WMQ</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:44:25</t>
+  </si>
+  <si>
+    <t>M9WMT</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:45:18</t>
+  </si>
+  <si>
+    <t>M9WMX</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:45:23</t>
+  </si>
+  <si>
+    <t>M9WMZ</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:45:35</t>
+  </si>
+  <si>
+    <t>M9WN5</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:46:18</t>
+  </si>
+  <si>
+    <t>M9WN6</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:46:25</t>
+  </si>
+  <si>
+    <t>M9WNB</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:47:10</t>
+  </si>
+  <si>
+    <t>M9WNG</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:47:37</t>
+  </si>
+  <si>
+    <t>M9WNQ</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:48:53</t>
+  </si>
+  <si>
+    <t>M9WNV</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:49:45</t>
+  </si>
+  <si>
+    <t>M9WNX</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:49:53</t>
+  </si>
+  <si>
+    <t>M9WNZ</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:49:59</t>
+  </si>
+  <si>
+    <t>M9WPF</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:50:45</t>
+  </si>
+  <si>
+    <t>M9WPH</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:50:51</t>
+  </si>
+  <si>
+    <t>M9WPN</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:51:03</t>
+  </si>
+  <si>
+    <t>M9WPZ</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:51:54</t>
+  </si>
+  <si>
+    <t>M9WQL</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:52:24</t>
+  </si>
+  <si>
+    <t>M9WQR</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:53:01</t>
+  </si>
+  <si>
+    <t>M9WQN</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:53:13</t>
+  </si>
+  <si>
+    <t>M9WQX</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:53:43</t>
+  </si>
+  <si>
+    <t>M9WQW</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:53:45</t>
+  </si>
+  <si>
+    <t>M9WR2</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:54:10</t>
+  </si>
+  <si>
+    <t>M9WR9</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:54:47</t>
+  </si>
+  <si>
+    <t>M9WRB</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:54:59</t>
+  </si>
+  <si>
+    <t>M9WRF</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:55:14</t>
+  </si>
+  <si>
+    <t>M9WRG</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:55:50</t>
+  </si>
+  <si>
+    <t>M9WRL</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:55:51</t>
+  </si>
+  <si>
+    <t>M9WRS</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:56:11</t>
+  </si>
+  <si>
+    <t>M9WRM</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:56:19</t>
+  </si>
+  <si>
+    <t>M9WS6</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:56:33</t>
+  </si>
+  <si>
+    <t>M9WS7</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:56:48</t>
+  </si>
+  <si>
+    <t>M9WSC</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:56:52</t>
+  </si>
+  <si>
+    <t>M9WSK</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:57:25</t>
+  </si>
+  <si>
+    <t>M9WSM</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:57:36</t>
+  </si>
+  <si>
+    <t>M9WSN</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:57:57</t>
+  </si>
+  <si>
+    <t>M9WST</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:58:16</t>
+  </si>
+  <si>
+    <t>M9WSV</t>
+  </si>
+  <si>
+    <t>M9WT3</t>
+  </si>
+  <si>
+    <t>3/2/2025, 8:59:23</t>
+  </si>
+  <si>
+    <t>M9WT5</t>
+  </si>
+  <si>
+    <t>M9WT6</t>
+  </si>
+  <si>
+    <t>3/2/2025, 9:00:10</t>
+  </si>
+  <si>
+    <t>M9WT8</t>
+  </si>
+  <si>
+    <t>3/2/2025, 9:00:26</t>
+  </si>
+  <si>
+    <t>M9WTM</t>
+  </si>
+  <si>
+    <t>3/2/2025, 9:01:12</t>
+  </si>
+  <si>
+    <t>M9WTV</t>
+  </si>
+  <si>
+    <t>3/2/2025, 9:02:05</t>
+  </si>
+  <si>
+    <t>M9WVK</t>
+  </si>
+  <si>
+    <t>3/2/2025, 9:02:28</t>
+  </si>
+  <si>
+    <t>M9WXS</t>
+  </si>
+  <si>
+    <t>3/2/2025, 9:04:30</t>
+  </si>
+  <si>
+    <t>M9XV2</t>
+  </si>
+  <si>
+    <t>3/2/2025, 9:29:48</t>
+  </si>
+  <si>
+    <t>H90C3</t>
+  </si>
+  <si>
+    <t>3/2/2025, 12:13:20</t>
+  </si>
+  <si>
+    <t>H90CD</t>
+  </si>
+  <si>
+    <t>3/2/2025, 12:14:24</t>
+  </si>
+  <si>
+    <t>H90M9</t>
+  </si>
+  <si>
+    <t>3/2/2025, 12:37:26</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,13 +386,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,31 +725,467 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Booking Code</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Date</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>LCJFM</v>
-      </c>
-      <c r="B2" t="str">
-        <v>30/1/2025, 13:01:42</v>
+    <row r="1" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
+    <ignoredError sqref="A1:B1 A2:B56" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
arregado lo del pais
</commit_message>
<xml_diff>
--- a/booking_codes.xlsx
+++ b/booking_codes.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z14"/>
+  <dimension ref="A1:AK18"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -481,6 +481,39 @@
       <c r="Z1" t="str">
         <v>Adult 1 Assistance</v>
       </c>
+      <c r="AA1" t="str">
+        <v>Outbound Flight Number</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>Outbound Departure Date</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>Outbound Departure Time</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>Outbound Arrival Date</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>Outbound Arrival Time</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>Outbound Duration</v>
+      </c>
+      <c r="AG1" t="str">
+        <v>Child 1 Name</v>
+      </c>
+      <c r="AH1" t="str">
+        <v>Child 1 Surname</v>
+      </c>
+      <c r="AI1" t="str">
+        <v>Child 1 Age</v>
+      </c>
+      <c r="AJ1" t="str">
+        <v>Child 1 Nationality</v>
+      </c>
+      <c r="AK1" t="str">
+        <v>Child 1 Assistance</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -655,9 +688,368 @@
         <v/>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>MEKEC</v>
+      </c>
+      <c r="C15" t="str">
+        <v>5/3/2025, 12:41:51</v>
+      </c>
+      <c r="D15" t="str">
+        <v>SCL</v>
+      </c>
+      <c r="E15" t="str">
+        <v>BCN</v>
+      </c>
+      <c r="F15" t="str">
+        <v>One Way</v>
+      </c>
+      <c r="G15" t="str">
+        <v>Economy</v>
+      </c>
+      <c r="H15" t="str">
+        <v>Light</v>
+      </c>
+      <c r="I15" t="str">
+        <v>Economy</v>
+      </c>
+      <c r="J15" t="str">
+        <v>Light</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15" t="str">
+        <v>EN</v>
+      </c>
+      <c r="O15" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="P15" t="str">
+        <v>Perez</v>
+      </c>
+      <c r="Q15" t="str">
+        <v>sofiainkoova@gmail.com</v>
+      </c>
+      <c r="R15" t="str">
+        <v>+93 791234567</v>
+      </c>
+      <c r="S15" t="str">
+        <v>2222 4000 7000 0005</v>
+      </c>
+      <c r="T15" t="str">
+        <v>Juan Pablo Antonio Maximiliano Alejandro Fernández de Córdoba Sánchez</v>
+      </c>
+      <c r="U15" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="V15" t="str">
+        <v>Perez</v>
+      </c>
+      <c r="W15" t="str">
+        <v>15</v>
+      </c>
+      <c r="X15" t="str">
+        <v>Afghanistan</v>
+      </c>
+      <c r="Y15" t="str">
+        <v>Female</v>
+      </c>
+      <c r="Z15" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>MEKH2</v>
+      </c>
+      <c r="C16" t="str">
+        <v>5/3/2025, 12:51:51</v>
+      </c>
+      <c r="D16" t="str">
+        <v>SCL</v>
+      </c>
+      <c r="E16" t="str">
+        <v>BCN</v>
+      </c>
+      <c r="F16" t="str">
+        <v>One Way</v>
+      </c>
+      <c r="G16" t="str">
+        <v>Economy</v>
+      </c>
+      <c r="H16" t="str">
+        <v>Light</v>
+      </c>
+      <c r="I16" t="str">
+        <v>Economy</v>
+      </c>
+      <c r="J16" t="str">
+        <v>Light</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16" t="str">
+        <v>EN</v>
+      </c>
+      <c r="O16" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="P16" t="str">
+        <v>Perez</v>
+      </c>
+      <c r="Q16" t="str">
+        <v>sofiainkoova@gmail.com</v>
+      </c>
+      <c r="R16" t="str">
+        <v>+93 791234567</v>
+      </c>
+      <c r="S16" t="str">
+        <v>2222 4000 7000 0005</v>
+      </c>
+      <c r="T16" t="str">
+        <v>Juan Pablo Antonio Maximiliano Alejandro Fernández de Córdoba Sánchez</v>
+      </c>
+      <c r="U16" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="V16" t="str">
+        <v>Perez</v>
+      </c>
+      <c r="W16" t="str">
+        <v>15</v>
+      </c>
+      <c r="X16" t="str">
+        <v>Afghanistan</v>
+      </c>
+      <c r="Y16" t="str">
+        <v>Female</v>
+      </c>
+      <c r="Z16" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>MEKMJ</v>
+      </c>
+      <c r="C17" t="str">
+        <v>5/3/2025, 13:01:48</v>
+      </c>
+      <c r="D17" t="str">
+        <v>SCL</v>
+      </c>
+      <c r="E17" t="str">
+        <v>BCN</v>
+      </c>
+      <c r="F17" t="str">
+        <v>One Way</v>
+      </c>
+      <c r="G17" t="str">
+        <v>Economy</v>
+      </c>
+      <c r="H17" t="str">
+        <v>Light</v>
+      </c>
+      <c r="I17" t="str">
+        <v>Economy</v>
+      </c>
+      <c r="J17" t="str">
+        <v>Light</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17" t="str">
+        <v>EN</v>
+      </c>
+      <c r="O17" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="P17" t="str">
+        <v>Perez</v>
+      </c>
+      <c r="Q17" t="str">
+        <v>sofiainkoova@gmail.com</v>
+      </c>
+      <c r="R17" t="str">
+        <v>+93 791234567</v>
+      </c>
+      <c r="S17" t="str">
+        <v>2222 4000 7000 0005</v>
+      </c>
+      <c r="T17" t="str">
+        <v>Juan Pablo Antonio Maximiliano Alejandro Fernández de Córdoba Sánchez</v>
+      </c>
+      <c r="U17" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="V17" t="str">
+        <v>Perez</v>
+      </c>
+      <c r="W17" t="str">
+        <v>15</v>
+      </c>
+      <c r="X17" t="str">
+        <v>Afghanistan</v>
+      </c>
+      <c r="Y17" t="str">
+        <v>Female</v>
+      </c>
+      <c r="Z17" t="str">
+        <v/>
+      </c>
+      <c r="AA17" t="str">
+        <v/>
+      </c>
+      <c r="AB17" t="str">
+        <v/>
+      </c>
+      <c r="AC17" t="str">
+        <v/>
+      </c>
+      <c r="AD17" t="str">
+        <v/>
+      </c>
+      <c r="AE17" t="str">
+        <v/>
+      </c>
+      <c r="AF17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>MEKQE</v>
+      </c>
+      <c r="C18" t="str">
+        <v>5/3/2025, 13:13:15</v>
+      </c>
+      <c r="D18" t="str">
+        <v>SCL</v>
+      </c>
+      <c r="E18" t="str">
+        <v>BCN</v>
+      </c>
+      <c r="F18" t="str">
+        <v>One Way</v>
+      </c>
+      <c r="G18" t="str">
+        <v>Economy</v>
+      </c>
+      <c r="H18" t="str">
+        <v>Light</v>
+      </c>
+      <c r="I18" t="str">
+        <v>Economy</v>
+      </c>
+      <c r="J18" t="str">
+        <v>Light</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18" t="str">
+        <v>EN</v>
+      </c>
+      <c r="O18" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="P18" t="str">
+        <v>Perez</v>
+      </c>
+      <c r="Q18" t="str">
+        <v>sofiainkoova@gmail.com</v>
+      </c>
+      <c r="R18" t="str">
+        <v>+93 791234567</v>
+      </c>
+      <c r="S18" t="str">
+        <v>5555 4444 3333 1111</v>
+      </c>
+      <c r="T18" t="str">
+        <v>Test Consumer</v>
+      </c>
+      <c r="U18" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="V18" t="str">
+        <v>Perez</v>
+      </c>
+      <c r="W18" t="str">
+        <v>15</v>
+      </c>
+      <c r="X18" t="str">
+        <v>Afghanistan</v>
+      </c>
+      <c r="Y18" t="str">
+        <v>Female</v>
+      </c>
+      <c r="Z18" t="str">
+        <v/>
+      </c>
+      <c r="AA18" t="str">
+        <v/>
+      </c>
+      <c r="AB18" t="str">
+        <v/>
+      </c>
+      <c r="AC18" t="str">
+        <v/>
+      </c>
+      <c r="AD18" t="str">
+        <v/>
+      </c>
+      <c r="AE18" t="str">
+        <v/>
+      </c>
+      <c r="AF18" t="str">
+        <v/>
+      </c>
+      <c r="AG18" t="str">
+        <v>Mateo</v>
+      </c>
+      <c r="AH18" t="str">
+        <v>Ramírez</v>
+      </c>
+      <c r="AI18" t="str">
+        <v>11</v>
+      </c>
+      <c r="AJ18" t="str">
+        <v>Argentina</v>
+      </c>
+      <c r="AK18" t="str">
+        <v>Visual difficulty</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Z14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AK18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
guardar informacion del vuelo
</commit_message>
<xml_diff>
--- a/booking_codes.xlsx
+++ b/booking_codes.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK18"/>
+  <dimension ref="A1:BA21"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -514,6 +514,54 @@
       <c r="AK1" t="str">
         <v>Child 1 Assistance</v>
       </c>
+      <c r="AL1" t="str">
+        <v>Outbound Flight Date</v>
+      </c>
+      <c r="AM1" t="str">
+        <v>Outbound Origin Code</v>
+      </c>
+      <c r="AN1" t="str">
+        <v>Outbound Origin Name</v>
+      </c>
+      <c r="AO1" t="str">
+        <v>Outbound Destination Code</v>
+      </c>
+      <c r="AP1" t="str">
+        <v>Outbound Destination Name</v>
+      </c>
+      <c r="AQ1" t="str">
+        <v>Outbound Arrival Next Day</v>
+      </c>
+      <c r="AR1" t="str">
+        <v>Outbound Airline</v>
+      </c>
+      <c r="AS1" t="str">
+        <v>Outbound Price</v>
+      </c>
+      <c r="AT1" t="str">
+        <v>Outbound Direction</v>
+      </c>
+      <c r="AU1" t="str">
+        <v>Outbound Selected Class</v>
+      </c>
+      <c r="AV1" t="str">
+        <v>Outbound Selected Type</v>
+      </c>
+      <c r="AW1" t="str">
+        <v>Outbound Cabin</v>
+      </c>
+      <c r="AX1" t="str">
+        <v>Outbound Economy Option</v>
+      </c>
+      <c r="AY1" t="str">
+        <v>Outbound Economy Price</v>
+      </c>
+      <c r="AZ1" t="str">
+        <v>Outbound Premium Option</v>
+      </c>
+      <c r="BA1" t="str">
+        <v>Outbound Premium Price</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -1047,9 +1095,381 @@
         <v>Visual difficulty</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>MEKTX</v>
+      </c>
+      <c r="C19" t="str">
+        <v>5/3/2025, 13:28:19</v>
+      </c>
+      <c r="D19" t="str">
+        <v>SCL</v>
+      </c>
+      <c r="E19" t="str">
+        <v>BCN</v>
+      </c>
+      <c r="F19" t="str">
+        <v>One Way</v>
+      </c>
+      <c r="G19" t="str">
+        <v>Economy</v>
+      </c>
+      <c r="H19" t="str">
+        <v>OUTBOUND</v>
+      </c>
+      <c r="I19" t="str">
+        <v>Economy</v>
+      </c>
+      <c r="J19" t="str">
+        <v>Light</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19" t="str">
+        <v>EN</v>
+      </c>
+      <c r="O19" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="P19" t="str">
+        <v>Perez</v>
+      </c>
+      <c r="Q19" t="str">
+        <v>sofiainkoova@gmail.com</v>
+      </c>
+      <c r="R19" t="str">
+        <v>+93 791234567</v>
+      </c>
+      <c r="S19" t="str">
+        <v>2222 4000 7000 0005</v>
+      </c>
+      <c r="T19" t="str">
+        <v>Juan Pablo Antonio Maximiliano Alejandro Fernández de Córdoba Sánchez</v>
+      </c>
+      <c r="U19" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="V19" t="str">
+        <v>Perez</v>
+      </c>
+      <c r="W19" t="str">
+        <v>15</v>
+      </c>
+      <c r="X19" t="str">
+        <v>Afghanistan</v>
+      </c>
+      <c r="Y19" t="str">
+        <v>Female</v>
+      </c>
+      <c r="Z19" t="str">
+        <v/>
+      </c>
+      <c r="AC19" t="str">
+        <v>10:25</v>
+      </c>
+      <c r="AE19" t="str">
+        <v>06:10</v>
+      </c>
+      <c r="AF19" t="str">
+        <v>13h 45m</v>
+      </c>
+      <c r="AL19" t="str">
+        <v>Tue, Jul 8</v>
+      </c>
+      <c r="AM19" t="str">
+        <v>SCL</v>
+      </c>
+      <c r="AN19" t="str">
+        <v>Santiago</v>
+      </c>
+      <c r="AO19" t="str">
+        <v>BCN</v>
+      </c>
+      <c r="AP19" t="str">
+        <v>Barcelona</v>
+      </c>
+      <c r="AQ19" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="AR19" t="str">
+        <v>IB</v>
+      </c>
+      <c r="AS19" t="str">
+        <v>$601</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>MEKX4</v>
+      </c>
+      <c r="C20" t="str">
+        <v>5/3/2025, 13:38:20</v>
+      </c>
+      <c r="D20" t="str">
+        <v>SCL</v>
+      </c>
+      <c r="E20" t="str">
+        <v>BCN</v>
+      </c>
+      <c r="F20" t="str">
+        <v>One Way</v>
+      </c>
+      <c r="G20" t="str">
+        <v>Economy</v>
+      </c>
+      <c r="H20" t="str">
+        <v>Light</v>
+      </c>
+      <c r="I20" t="str">
+        <v>Economy</v>
+      </c>
+      <c r="J20" t="str">
+        <v>Light</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20" t="str">
+        <v>EN</v>
+      </c>
+      <c r="O20" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="P20" t="str">
+        <v>Perez</v>
+      </c>
+      <c r="Q20" t="str">
+        <v>sofiainkoova@gmail.com</v>
+      </c>
+      <c r="R20" t="str">
+        <v>+93 791234567</v>
+      </c>
+      <c r="S20" t="str">
+        <v>2222 4000 7000 0005</v>
+      </c>
+      <c r="T20" t="str">
+        <v>Juan Pablo Antonio Maximiliano Alejandro Fernández de Córdoba Sánchez</v>
+      </c>
+      <c r="U20" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="V20" t="str">
+        <v>Perez</v>
+      </c>
+      <c r="W20" t="str">
+        <v>15</v>
+      </c>
+      <c r="X20" t="str">
+        <v>Afghanistan</v>
+      </c>
+      <c r="Y20" t="str">
+        <v>Female</v>
+      </c>
+      <c r="Z20" t="str">
+        <v/>
+      </c>
+      <c r="AC20" t="str">
+        <v>10:25</v>
+      </c>
+      <c r="AE20" t="str">
+        <v>06:10</v>
+      </c>
+      <c r="AF20" t="str">
+        <v>13h 45m</v>
+      </c>
+      <c r="AL20" t="str">
+        <v>Tue, Jul 29</v>
+      </c>
+      <c r="AM20" t="str">
+        <v>SCL</v>
+      </c>
+      <c r="AN20" t="str">
+        <v>Santiago</v>
+      </c>
+      <c r="AO20" t="str">
+        <v>BCN</v>
+      </c>
+      <c r="AP20" t="str">
+        <v>Barcelona</v>
+      </c>
+      <c r="AQ20" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="AR20" t="str">
+        <v>IB</v>
+      </c>
+      <c r="AT20" t="str">
+        <v>OUTBOUND</v>
+      </c>
+      <c r="AU20" t="str">
+        <v>Economy</v>
+      </c>
+      <c r="AV20" t="str">
+        <v>Light</v>
+      </c>
+      <c r="AW20" t="str">
+        <v>Economy Light</v>
+      </c>
+      <c r="AX20" t="str">
+        <v>ECONOMY</v>
+      </c>
+      <c r="AY20" t="str">
+        <v>$565</v>
+      </c>
+      <c r="AZ20" t="str">
+        <v>PREMIUM</v>
+      </c>
+      <c r="BA20" t="str">
+        <v>$751</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>MEKZG</v>
+      </c>
+      <c r="C21" t="str">
+        <v>5/3/2025, 13:46:13</v>
+      </c>
+      <c r="D21" t="str">
+        <v>SCL</v>
+      </c>
+      <c r="E21" t="str">
+        <v>BCN</v>
+      </c>
+      <c r="F21" t="str">
+        <v>One Way</v>
+      </c>
+      <c r="G21" t="str">
+        <v>Economy</v>
+      </c>
+      <c r="H21" t="str">
+        <v>Light</v>
+      </c>
+      <c r="I21" t="str">
+        <v>Economy</v>
+      </c>
+      <c r="J21" t="str">
+        <v>Light</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21" t="str">
+        <v>EN</v>
+      </c>
+      <c r="O21" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="P21" t="str">
+        <v>Perez</v>
+      </c>
+      <c r="Q21" t="str">
+        <v>sofiainkoova@gmail.com</v>
+      </c>
+      <c r="R21" t="str">
+        <v>+93 791234567</v>
+      </c>
+      <c r="S21" t="str">
+        <v>2222 4000 7000 0005</v>
+      </c>
+      <c r="T21" t="str">
+        <v>Juan Pablo Antonio Maximiliano Alejandro Fernández de Córdoba Sánchez</v>
+      </c>
+      <c r="U21" t="str">
+        <v>Juan</v>
+      </c>
+      <c r="V21" t="str">
+        <v>Perez</v>
+      </c>
+      <c r="W21" t="str">
+        <v>15</v>
+      </c>
+      <c r="X21" t="str">
+        <v>Afghanistan</v>
+      </c>
+      <c r="Y21" t="str">
+        <v>Female</v>
+      </c>
+      <c r="Z21" t="str">
+        <v/>
+      </c>
+      <c r="AC21" t="str">
+        <v>10:25</v>
+      </c>
+      <c r="AE21" t="str">
+        <v>06:10</v>
+      </c>
+      <c r="AF21" t="str">
+        <v>13h 45m</v>
+      </c>
+      <c r="AL21" t="str">
+        <v>Tue, Jul 8</v>
+      </c>
+      <c r="AM21" t="str">
+        <v>SCL</v>
+      </c>
+      <c r="AN21" t="str">
+        <v>Santiago</v>
+      </c>
+      <c r="AO21" t="str">
+        <v>BCN</v>
+      </c>
+      <c r="AP21" t="str">
+        <v>Barcelona</v>
+      </c>
+      <c r="AQ21" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="AR21" t="str">
+        <v>IB</v>
+      </c>
+      <c r="AT21" t="str">
+        <v>OUTBOUND</v>
+      </c>
+      <c r="AU21" t="str">
+        <v>Economy</v>
+      </c>
+      <c r="AV21" t="str">
+        <v>Light</v>
+      </c>
+      <c r="AW21" t="str">
+        <v>Economy Light</v>
+      </c>
+      <c r="AX21" t="str">
+        <v>ECONOMY</v>
+      </c>
+      <c r="AY21" t="str">
+        <v>$601</v>
+      </c>
+      <c r="AZ21" t="str">
+        <v>PREMIUM</v>
+      </c>
+      <c r="BA21" t="str">
+        <v>$751</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AK18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:BA21"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>